<commit_message>
Review report + corrections
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bubu_\Desktop\VVSS\Docs\Lab01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D7150A-ED81-43DE-8340-5C435FFACFCF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
     <sheet name="Architect. Design Phase Defects" sheetId="6" r:id="rId2"/>
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -76,12 +82,72 @@
   </si>
   <si>
     <t>Review Form. Requirements Defects</t>
+  </si>
+  <si>
+    <t>Bulmez Alexandru - Florin</t>
+  </si>
+  <si>
+    <t>03.18.2019</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R1,R2</t>
+  </si>
+  <si>
+    <t>par 1</t>
+  </si>
+  <si>
+    <t>par 5</t>
+  </si>
+  <si>
+    <t>Nu se precizeaza conditia conform careia un elev este considerat corigent la o materie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nu se precizeaza tipul de aplicatie  (aplicatie consola sau aplicatie cu interfata grafica)</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>Nu, lipsesc anumite concepte: conceptul de Nota</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>Nu, desi prezenta in diagrama, clasa ClasaException nu este utilizata (conform relatiilor dintre clase)</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>Nu, lipseste stratul de UI din cadrul unei arhitecturi stratificate</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>Clasa ClasaException este importata gresit in cadrul claselor StartApp, AddNotaTest, CalculeazaMediiTest, GetCorigentiTest, IntegrationTest, NoteController</t>
+  </si>
+  <si>
+    <t>Lipsa fisierelor de intrare pentru elevi si note</t>
+  </si>
+  <si>
+    <t>In cadrul clasei Elev campul nrmatricol este de tip int, pe cand in cadrul clasei Nota campul nrmatricol este de tip double</t>
+  </si>
+  <si>
+    <t>Nu se precizeaza formatul si numele fisierelor de intrare</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,7 +312,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -257,6 +322,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -299,6 +365,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -347,7 +416,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -380,9 +449,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -415,6 +501,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -590,7 +693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
@@ -600,22 +703,22 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>19</v>
       </c>
@@ -623,8 +726,8 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="14" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -632,8 +735,8 @@
       </c>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="14" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="21" t="s">
@@ -641,22 +744,26 @@
       </c>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -666,37 +773,55 @@
       <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -705,7 +830,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -714,7 +839,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -723,7 +848,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -732,7 +857,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -741,87 +866,86 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="12" t="s">
+      <c r="E25" s="15"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="1"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="17">
+        <v>2.0833333333333332E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -837,32 +961,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>18</v>
       </c>
@@ -870,7 +994,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -879,7 +1003,7 @@
       </c>
       <c r="E4" s="23"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -888,22 +1012,26 @@
       </c>
       <c r="E5" s="25"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -917,33 +1045,45 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E11" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -952,7 +1092,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -961,7 +1101,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -970,7 +1110,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -979,7 +1119,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -988,7 +1128,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -997,7 +1137,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1006,7 +1146,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1015,7 +1155,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1024,7 +1164,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1033,7 +1173,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1042,7 +1182,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1051,7 +1191,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1060,7 +1200,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1069,15 +1209,14 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="12" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="E28" s="1"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="17">
+        <v>2.0833333333333332E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1093,33 +1232,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="6"/>
+    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="16384" width="8.89453125" style="6"/>
+    <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>17</v>
       </c>
@@ -1127,8 +1266,8 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="17" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="26" t="s">
@@ -1136,8 +1275,8 @@
       </c>
       <c r="E4" s="26"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="17" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="27" t="s">
@@ -1145,22 +1284,26 @@
       </c>
       <c r="E5" s="28"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="20" t="s">
+        <v>21</v>
+      </c>
       <c r="E7" s="20"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1174,33 +1317,45 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E12" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1209,7 +1364,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1218,7 +1373,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1227,7 +1382,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1236,7 +1391,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1245,7 +1400,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1254,7 +1409,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1263,7 +1418,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1272,7 +1427,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1281,7 +1436,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1290,7 +1445,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1299,7 +1454,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1308,7 +1463,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1317,7 +1472,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1326,7 +1481,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1335,7 +1490,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1344,7 +1499,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1353,7 +1508,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1362,15 +1517,14 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C32" s="12" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="1"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="17">
+        <v>4.1666666666666664E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>